<commit_message>
Added excel export functionality (amongst other things)
</commit_message>
<xml_diff>
--- a/resources/documents/placeholder.xlsx
+++ b/resources/documents/placeholder.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="48" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{886E0B0E-9376-4156-A2B9-5EF014226A88}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackhayley/Documents/GitHub/PTTech/Quote-Assistant/resources/documents/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D9905D-285D-2B42-A92C-1EA84FFC9E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="100" windowWidth="23660" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,8 +68,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -107,12 +123,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,69 +448,69 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="1"/>
+      <c r="H1" s="4"/>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
       <c r="H3" s="2"/>
     </row>
   </sheetData>

</xml_diff>